<commit_message>
update - new notebook running the model
</commit_message>
<xml_diff>
--- a/data/co2_tax.xlsx
+++ b/data/co2_tax.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://dtudk-my.sharepoint.com/personal/s203679_dtu_dk/Documents/Dokumenter/DTU_Man/h2_system_dynamics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{4565646E-C921-4C53-B13C-ED99545D5B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A12007B5-5BD0-4F2D-AADD-D23B6C841AFA}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="8_{4565646E-C921-4C53-B13C-ED99545D5B41}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8AD080D3-0636-49B0-AFB9-9F51F6C58A37}"/>
   <bookViews>
-    <workbookView xWindow="-19310" yWindow="-110" windowWidth="19420" windowHeight="11020" xr2:uid="{BA38977B-D26D-488D-AA4F-B91484DAE233}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{BA38977B-D26D-488D-AA4F-B91484DAE233}"/>
   </bookViews>
   <sheets>
     <sheet name="co2 tax" sheetId="1" r:id="rId1"/>
@@ -413,7 +413,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E936772-280D-4228-8295-B8F62D458075}">
-  <dimension ref="A1:N40"/>
+  <dimension ref="A1:B40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N12" sqref="N12"/>
@@ -424,7 +424,7 @@
     <col min="14" max="14" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -432,7 +432,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2012</v>
       </c>
@@ -440,7 +440,7 @@
         <v>7.59</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2013</v>
       </c>
@@ -448,7 +448,7 @@
         <v>4.8499999999999996</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2014</v>
       </c>
@@ -456,7 +456,7 @@
         <v>6.35</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2015</v>
       </c>
@@ -464,7 +464,7 @@
         <v>7.49</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2016</v>
       </c>
@@ -472,7 +472,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2017</v>
       </c>
@@ -480,7 +480,7 @@
         <v>5.79</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2018</v>
       </c>
@@ -488,7 +488,7 @@
         <v>5.95</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2019</v>
       </c>
@@ -496,7 +496,7 @@
         <v>14.26</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2020</v>
       </c>
@@ -504,7 +504,7 @@
         <v>22.57</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2021</v>
       </c>
@@ -512,19 +512,15 @@
         <v>48.152999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2022</v>
       </c>
       <c r="B12">
         <v>54.870165155555554</v>
       </c>
-      <c r="N12">
-        <f>1.5*16.2/8.7</f>
-        <v>2.7931034482758621</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2023</v>
       </c>
@@ -532,7 +528,7 @@
         <v>61.58733031111111</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2024</v>
       </c>
@@ -540,7 +536,7 @@
         <v>68.304495466666665</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2025</v>
       </c>
@@ -548,7 +544,7 @@
         <v>75.021660622222228</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2026</v>
       </c>

</xml_diff>